<commit_message>
added hints to excel
</commit_message>
<xml_diff>
--- a/Assets/Pictures_Info.xlsx
+++ b/Assets/Pictures_Info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Downloads\GeoGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\FHNW\60 Projekte\68 - GIT WEBEC Modulprojekt GeoGame\geogame\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
   <si>
     <t>001</t>
   </si>
@@ -122,9 +122,6 @@
     <t>picture_Location</t>
   </si>
   <si>
-    <t>picture_Coordinates</t>
-  </si>
-  <si>
     <t>picture_Name</t>
   </si>
   <si>
@@ -188,12 +185,6 @@
     <t>Lupfig</t>
   </si>
   <si>
-    <t>Grossratsgebäude Aargau</t>
-  </si>
-  <si>
-    <t>Feldschlössche AG</t>
-  </si>
-  <si>
     <t>Grand Hotel Dolder</t>
   </si>
   <si>
@@ -377,94 +368,82 @@
     <t>GeoGame_Picture_030</t>
   </si>
   <si>
-    <t>47.533972, 7.721350</t>
-  </si>
-  <si>
-    <t>46.947967, 7.447776</t>
-  </si>
-  <si>
-    <t>47.476105, 8.213079</t>
-  </si>
-  <si>
-    <t>47.349513, 8.491128</t>
-  </si>
-  <si>
-    <t>47.339778, 8.051690</t>
-  </si>
-  <si>
-    <t>46.947967, 7.450432</t>
-  </si>
-  <si>
-    <t>47.473099, 8.305553</t>
-  </si>
-  <si>
-    <t>47.186581,8.400497</t>
-  </si>
-  <si>
-    <t>47.350269, 8.340306</t>
-  </si>
-  <si>
-    <t>47.351694, 8.277931</t>
-  </si>
-  <si>
-    <t>47.369746, 8.538941</t>
-  </si>
-  <si>
-    <t>47.275300, 8.337912</t>
-  </si>
-  <si>
-    <t>47.320590, 7.899009</t>
-  </si>
-  <si>
-    <t>47.051627, 8.307542</t>
-  </si>
-  <si>
-    <t>47.355808, 8.270453</t>
-  </si>
-  <si>
-    <t>47.454906, 8.311795</t>
-  </si>
-  <si>
-    <t>47.389641, 8.045520</t>
-  </si>
-  <si>
-    <t>47.372669, 8.573137</t>
-  </si>
-  <si>
-    <t>47.443837, 8.229625</t>
-  </si>
-  <si>
-    <t>47.481693, 8.210857</t>
-  </si>
-  <si>
-    <t>47.546603, 7.785562</t>
-  </si>
-  <si>
-    <t>47.376514, 8.548349</t>
-  </si>
-  <si>
-    <t>46.946843, 7.444167</t>
-  </si>
-  <si>
-    <t>47.378311, 8.539212</t>
-  </si>
-  <si>
-    <t>47.480940, 8.208648</t>
-  </si>
-  <si>
-    <t>47.476394, 8.307915</t>
-  </si>
-  <si>
-    <t>47.396791, 8.242088</t>
-  </si>
-  <si>
-    <t>47.393242, 8.053227</t>
-  </si>
-  <si>
-    <t>47.288591, 7.946121</t>
-  </si>
-  <si>
-    <t>47.350476, 8.245703</t>
+    <t>Kantonsschule</t>
+  </si>
+  <si>
+    <t>Bahnhof</t>
+  </si>
+  <si>
+    <t>Kloster</t>
+  </si>
+  <si>
+    <t>Reussbrücke</t>
+  </si>
+  <si>
+    <t>Ruine</t>
+  </si>
+  <si>
+    <t>Regierungsgebäude</t>
+  </si>
+  <si>
+    <t>Aussichtsturm</t>
+  </si>
+  <si>
+    <t>Pfarrkirche</t>
+  </si>
+  <si>
+    <t>Hochschule</t>
+  </si>
+  <si>
+    <t>Feldschlösschen AG</t>
+  </si>
+  <si>
+    <t>Brunnen</t>
+  </si>
+  <si>
+    <t>Reformierte Kirche</t>
+  </si>
+  <si>
+    <t>"Frisch vom Schloss"</t>
+  </si>
+  <si>
+    <t>Ehemaliges Römerlager</t>
+  </si>
+  <si>
+    <t>Bekannteste Uhr der Schweiz</t>
+  </si>
+  <si>
+    <t>Endstation der Spanisch-Brötli-Bahn</t>
+  </si>
+  <si>
+    <t>Ehemaliges Bundeshaus</t>
+  </si>
+  <si>
+    <t>Teuerstes Grundstück bei Monopoly Schweiz</t>
+  </si>
+  <si>
+    <t>Ältestes nichtkirchliches Gymnasium der Schweiz</t>
+  </si>
+  <si>
+    <t>Regionalflugplatz</t>
+  </si>
+  <si>
+    <t>Brücke über die Limmat</t>
+  </si>
+  <si>
+    <t>1993 niedergebrannt, 1994 wiedereröffnet</t>
+  </si>
+  <si>
+    <t>Beliebtes Naherholungsgebiet</t>
+  </si>
+  <si>
+    <t>5-Sterne Hotel</t>
+  </si>
+  <si>
+    <t>picture_Longitude</t>
+  </si>
+  <si>
+    <t>picture_Latitude</t>
   </si>
 </sst>
 </file>
@@ -517,10 +496,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -801,20 +786,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1048572"/>
+  <dimension ref="A1:G1048572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="40.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="5" width="20.6328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" customWidth="1"/>
+    <col min="7" max="7" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -822,526 +810,709 @@
         <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="D2" s="4">
+        <v>47.396791</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8.2420880000000007</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4">
+        <v>47.393242000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.0532269999999997</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="D4" s="4">
+        <v>47.476393999999999</v>
+      </c>
+      <c r="E4" s="4">
+        <v>8.3079149999999995</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4">
+        <v>47.480939999999997</v>
+      </c>
+      <c r="E5" s="4">
+        <v>8.2086480000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4">
+        <v>47.378310999999997</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8.5392119999999991</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4">
+        <v>46.946843000000001</v>
+      </c>
+      <c r="E7" s="4">
+        <v>7.4441670000000002</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="D8" s="4">
+        <v>47.376514</v>
+      </c>
+      <c r="E8" s="4">
+        <v>8.548349</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4">
+        <v>47.546602999999998</v>
+      </c>
+      <c r="E9" s="4">
+        <v>7.7855619999999996</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4">
+        <v>47.481693</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8.2108570000000007</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4">
+        <v>47.443837000000002</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8.2296250000000004</v>
+      </c>
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4">
+        <v>47.372669000000002</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8.5731369999999991</v>
+      </c>
+      <c r="F12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="D13" s="4">
+        <v>47.389640999999997</v>
+      </c>
+      <c r="E13" s="4">
+        <v>8.0455199999999998</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="D14" s="4">
+        <v>47.454906000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8.311795</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="D15" s="4">
+        <v>47.355808000000003</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8.2704529999999998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="D16" s="4">
+        <v>47.051627000000003</v>
+      </c>
+      <c r="E16" s="4">
+        <v>8.3075419999999998</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4">
+        <v>47.320590000000003</v>
+      </c>
+      <c r="E17" s="4">
+        <v>7.8990090000000004</v>
+      </c>
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4">
+        <v>47.275300000000001</v>
+      </c>
+      <c r="E18" s="4">
+        <v>8.3379119999999993</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4">
+        <v>47.369745999999999</v>
+      </c>
+      <c r="E19" s="4">
+        <v>8.5389409999999994</v>
+      </c>
+      <c r="F19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="D20" s="4">
+        <v>47.351694000000002</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8.2779310000000006</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="D21" s="4">
+        <v>47.350476</v>
+      </c>
+      <c r="E21" s="4">
+        <v>8.2457030000000007</v>
+      </c>
+      <c r="F21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="D22" s="4">
+        <v>47.350268999999997</v>
+      </c>
+      <c r="E22" s="4">
+        <v>8.340306</v>
+      </c>
+      <c r="F22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="D23" s="4">
+        <v>47.186580999999997</v>
+      </c>
+      <c r="E23" s="4">
+        <v>8.4004969999999997</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4">
+        <v>47.473098999999998</v>
+      </c>
+      <c r="E24" s="4">
+        <v>8.3055529999999997</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>122</v>
-      </c>
-      <c r="E25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="D25" s="4">
+        <v>46.947966999999998</v>
+      </c>
+      <c r="E25" s="4">
+        <v>7.4504320000000002</v>
+      </c>
+      <c r="F25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="D26" s="4">
+        <v>47.339778000000003</v>
+      </c>
+      <c r="E26" s="4">
+        <v>8.0516900000000007</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="D27" s="4">
+        <v>47.288590999999997</v>
+      </c>
+      <c r="E27" s="4">
+        <v>7.9461209999999998</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="D28" s="4">
+        <v>47.349513000000002</v>
+      </c>
+      <c r="E28" s="4">
+        <v>8.4911279999999998</v>
+      </c>
+      <c r="F28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="D29" s="4">
+        <v>47.476104999999997</v>
+      </c>
+      <c r="E29" s="4">
+        <v>8.2130790000000005</v>
+      </c>
+      <c r="F29" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="D30" s="4">
+        <v>46.947966999999998</v>
+      </c>
+      <c r="E30" s="4">
+        <v>7.4477760000000002</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" t="s">
-        <v>116</v>
+        <v>80</v>
+      </c>
+      <c r="D31" s="4">
+        <v>47.533971999999999</v>
+      </c>
+      <c r="E31" s="4">
+        <v>7.7213500000000002</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="1048572" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Changed some hints and added some features in the GUI
</commit_message>
<xml_diff>
--- a/Assets/Pictures_Info.xlsx
+++ b/Assets/Pictures_Info.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\FHNW\60 Projekte\68 - GIT WEBEC Modulprojekt GeoGame\geogame\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\workspace\GIT_Repositories\geogame\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="7750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
   <si>
     <t>001</t>
   </si>
@@ -392,9 +392,6 @@
     <t>Pfarrkirche</t>
   </si>
   <si>
-    <t>Hochschule</t>
-  </si>
-  <si>
     <t>Feldschlösschen AG</t>
   </si>
   <si>
@@ -444,12 +441,24 @@
   </si>
   <si>
     <t>picture_Latitude</t>
+  </si>
+  <si>
+    <t>Anfangssation fuhr der Spanisch-Brötli-Bahn!</t>
+  </si>
+  <si>
+    <t>Dieser Brunnen wurde dem Stadthelden von Zofingen gewidmet</t>
+  </si>
+  <si>
+    <t>Will man in die Forschung sollte man hier studieren</t>
+  </si>
+  <si>
+    <t>Hier kann man iCompetence studieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -788,21 +797,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1048572"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="5" width="20.6328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="25.6328125" customWidth="1"/>
-    <col min="7" max="7" width="50.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -813,10 +822,10 @@
         <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>32</v>
@@ -825,7 +834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +857,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -868,10 +877,10 @@
         <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -891,10 +900,10 @@
         <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -917,7 +926,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -937,10 +946,10 @@
         <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -963,7 +972,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -983,15 +992,15 @@
         <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
@@ -1006,10 +1015,10 @@
         <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1029,10 +1038,10 @@
         <v>92</v>
       </c>
       <c r="G10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1052,10 +1061,10 @@
         <v>93</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1075,10 +1084,10 @@
         <v>94</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1098,10 +1107,10 @@
         <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1121,10 +1130,10 @@
         <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1156,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1167,10 +1176,10 @@
         <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1190,10 +1199,10 @@
         <v>99</v>
       </c>
       <c r="G17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1236,10 +1245,10 @@
         <v>101</v>
       </c>
       <c r="G19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1262,7 +1271,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1282,10 +1291,10 @@
         <v>103</v>
       </c>
       <c r="G21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1331,7 +1340,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1374,10 +1383,10 @@
         <v>107</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1420,10 +1429,10 @@
         <v>109</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1443,10 +1452,10 @@
         <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1466,10 +1475,10 @@
         <v>111</v>
       </c>
       <c r="G29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1489,10 +1498,10 @@
         <v>112</v>
       </c>
       <c r="G30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1512,10 +1521,10 @@
         <v>113</v>
       </c>
       <c r="G31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="1048572" spans="1:1" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1048572" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1048572" s="1"/>
     </row>
   </sheetData>

</xml_diff>